<commit_message>
updated data workflow chapters
</commit_message>
<xml_diff>
--- a/data-dictionaries/dd-nptrends-wave-02.xlsx
+++ b/data-dictionaries/dd-nptrends-wave-02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdlec\Dropbox (Personal)\00 - URBAN\00-GITHUB\nccs-nptrends\data-dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4769FFFE-E72E-4295-84E4-B6E957498C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F0B522-ED19-4F2F-A7AB-10B40E3C93CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="48015" windowHeight="18495" activeTab="2" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
+    <workbookView xWindow="34290" yWindow="0" windowWidth="17415" windowHeight="20985" xr2:uid="{5572D8ED-434A-412A-A007-947EB1DCFE87}"/>
   </bookViews>
   <sheets>
     <sheet name="data dictionary" sheetId="2" r:id="rId1"/>
@@ -4176,9 +4176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EA05EC-8AD9-456D-B4A3-808D5594C485}">
   <dimension ref="A1:M226"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12237,13 +12237,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD8CABA-E2BC-451A-8F2B-D5B38142330D}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="19.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="27.77734375" style="6" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="6" customWidth="1"/>

</xml_diff>